<commit_message>
Application Foward and backward rotabit counter
</commit_message>
<xml_diff>
--- a/Doc/Requirements/Systems_Requirements.xlsx
+++ b/Doc/Requirements/Systems_Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dario/Documents/Freedom_Workspace/PracticaReproductorAudio/Doc/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5562F0CE-4BC7-0343-9A71-824475897EC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D8DB8F-C9A6-B446-AB55-5F57B48D4BA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27320" yWindow="460" windowWidth="25600" windowHeight="18660" xr2:uid="{F1874689-60D1-6845-B7F9-40A4A5597352}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BE9308-E0B3-B149-A6C0-ACA685B46976}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>